<commit_message>
[PHOENIX-5854] removed trade license tag for which automation tests were failing due to workflow changes
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/tradeLicenseTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/tradeLicenseTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8190" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="tradeOwnerDetails" sheetId="1" r:id="rId1"/>
@@ -48,15 +48,6 @@
     <t>123456789123</t>
   </si>
   <si>
-    <t>Bimal</t>
-  </si>
-  <si>
-    <t>Ajaya kumar</t>
-  </si>
-  <si>
-    <t>bimal@gmail.com</t>
-  </si>
-  <si>
     <t>Bangalore</t>
   </si>
   <si>
@@ -175,6 +166,15 @@
   </si>
   <si>
     <t>01/04/2017</t>
+  </si>
+  <si>
+    <t>Akhila</t>
+  </si>
+  <si>
+    <t>Divakar</t>
+  </si>
+  <si>
+    <t>abc@xyz.com</t>
   </si>
 </sst>
 </file>
@@ -192,17 +192,18 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,8 +223,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -240,19 +242,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -554,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -604,16 +607,16 @@
         <v>2222222222</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -639,47 +642,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="9"/>
-    <col min="2" max="2" width="24.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="9"/>
-    <col min="6" max="1027" width="11.28515625" style="9"/>
-    <col min="1028" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="20.28515625" style="8"/>
+    <col min="2" max="2" width="24.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="8"/>
+    <col min="6" max="1027" width="11.28515625" style="8"/>
+    <col min="1028" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>14</v>
+      <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -714,63 +717,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="C2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="E2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="6">
+        <v>100</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="7">
-        <v>100</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>51</v>
+      <c r="H2" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>44</v>
+      <c r="D4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -793,54 +796,54 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="9"/>
-    <col min="2" max="2" width="16.42578125" style="9"/>
-    <col min="3" max="1025" width="11.28515625" style="9"/>
+    <col min="1" max="1" width="13.7109375" style="8"/>
+    <col min="2" max="2" width="16.42578125" style="8"/>
+    <col min="3" max="1025" width="11.28515625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>10</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>20</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>30</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>40</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="8">
         <v>50</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="8">
         <v>60</v>
       </c>
     </row>
@@ -858,7 +861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -874,21 +877,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>35</v>
+      <c r="A2" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -913,26 +916,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>